<commit_message>
Fixed not sending INFORM ACL by the WorkCenterAgent
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView activeTab="3" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="ShopOrders" r:id="rId1" sheetId="1"/>
-    <sheet name="ShopOrderOperations" r:id="rId2" sheetId="2"/>
-    <sheet name="WorkCenters" r:id="rId3" sheetId="3"/>
-    <sheet name="WorkCenterOpAllocations" r:id="rId4" sheetId="4"/>
+    <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
+    <sheet name="ShopOrderOperations" sheetId="2" r:id="rId2"/>
+    <sheet name="WorkCenters" sheetId="3" r:id="rId3"/>
+    <sheet name="WorkCenterOpAllocations" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -222,19 +222,19 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
-    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -251,10 +251,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -289,7 +289,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -324,7 +324,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -418,21 +418,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -449,7 +449,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -501,15 +501,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
@@ -517,19 +517,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.85546875" collapsed="true"/>
-    <col min="3" max="4" customWidth="true" style="1" width="14.28515625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="17.28515625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="17.140625" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -615,14 +615,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
@@ -630,20 +630,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="13.7109375" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="22.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.140625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="13.5703125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="16.7109375" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -726,14 +726,14 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -741,10 +741,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="16.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -790,13 +790,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -804,8 +804,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.85546875" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,9 +930,6 @@
       <c r="B9" s="1">
         <v>43318</v>
       </c>
-      <c r="C9" t="n">
-        <v>1.0</v>
-      </c>
       <c r="J9">
         <v>2</v>
       </c>
@@ -1007,7 +1004,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DYNO-20: Update Best Date Offer logic of the Work Center Agent
Bug Fixes, code refactoring
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B03BF6-D878-4938-90AB-B17679D7FDB2}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB3737-9076-4963-892D-4B87581508AA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -669,7 +669,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -755,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -878,7 +878,7 @@
   <dimension ref="A1:AMK15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -928,7 +928,7 @@
         <v>43318</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>3</v>
@@ -1020,6 +1020,9 @@
       </c>
       <c r="B10" s="1">
         <v>43319</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
       </c>
       <c r="F10">
         <v>1</v>

</xml_diff>

<commit_message>
excel sheet data changes for testing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\Work\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FB3737-9076-4963-892D-4B87581508AA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D056621B-E09F-4BFF-8B6F-437890AEF1D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -558,25 +558,25 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.3046875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.84375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.3046875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.3828125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.15234375" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.69140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.15234375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.69140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -668,30 +668,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.69140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.69140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.69140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19.15234375" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.53515625" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.53515625" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.84375" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.15234375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.15234375" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.3828125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.69140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.3828125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.53515625" customWidth="1" collapsed="1"/>
+    <col min="16" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -755,7 +755,7 @@
         <v>1</v>
       </c>
       <c r="F2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -770,7 +770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -816,16 +816,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.3828125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.15234375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.84375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.3828125" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -839,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -853,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -877,18 +877,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.84375" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -920,7 +920,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -934,7 +934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -981,7 +981,7 @@
         <v>43322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -989,7 +989,7 @@
         <v>43323</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1052,8 +1052,11 @@
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1075,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
DYNO-19: Handle multiple Shop Order Scenario
Fixed locking mechanism issue with processing the operation queue.
Added a better locking mechanism with ReentrantLock.
Added methods to support Shop Order and Work Center communication for scheduling the operation. Should be implemented and tested.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\Work\DynoScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D056621B-E09F-4BFF-8B6F-437890AEF1D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E777EB2F-74A6-4BD2-8B08-8496B43EAE3F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -558,25 +558,25 @@
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.84375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="14.3046875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.3046875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.3828125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.15234375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.69140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.15234375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.69140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,7 +620,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -669,29 +669,29 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.69140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.69140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.69140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19.15234375" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.53515625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.53515625" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.84375" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.15234375" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.15234375" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.3828125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.69140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.69140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.3828125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.53515625" customWidth="1" collapsed="1"/>
-    <col min="16" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="16" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -738,7 +738,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -770,7 +770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -816,16 +816,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3828125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.15234375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.84375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.3828125" customWidth="1" collapsed="1"/>
-    <col min="5" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -839,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -853,7 +853,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -881,14 +881,14 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.84375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -920,7 +920,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -934,7 +934,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -962,7 +962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -981,7 +981,7 @@
         <v>43322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -989,7 +989,7 @@
         <v>43323</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1003,7 +1003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1028,7 +1028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1039,7 +1039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1056,7 +1056,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Changes to the Shop Order Operation table
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\Work\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F634DDF-DAFE-442D-8D49-24EC25D7082A}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91294EA2-5ADA-407E-BA88-F8D1F8D4412C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>OrderNo</t>
   </si>
@@ -199,6 +199,15 @@
   </si>
   <si>
     <t>op4</t>
+  </si>
+  <si>
+    <t>PrecedingOperation</t>
+  </si>
+  <si>
+    <t>WCRuntimeFactor</t>
+  </si>
+  <si>
+    <t>LaborRuntimeFactor</t>
   </si>
 </sst>
 </file>
@@ -566,29 +575,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.42578125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.3046875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.84375" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="14.3046875" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.3046875" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.3828125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.3828125" style="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.69140625" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.84375" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.15234375" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
-    <col min="15" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.69140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.15234375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.69140625" customWidth="1" collapsed="1"/>
+    <col min="15" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +641,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -670,7 +679,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>2</v>
       </c>
@@ -716,32 +725,34 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AMK5"/>
+  <dimension ref="A1:AMN5"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.140625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="11.85546875" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="12.140625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.140625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="13.42578125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.7109375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="16.7109375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1" collapsed="1"/>
-    <col min="16" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.69140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.69140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.69140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.15234375" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="20.15234375" customWidth="1"/>
+    <col min="8" max="8" width="19.53515625" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.53515625" customWidth="1"/>
+    <col min="10" max="10" width="13.53515625" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.84375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.15234375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.15234375" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.3828125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.69140625" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.3828125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.53515625" customWidth="1" collapsed="1"/>
+    <col min="19" max="1028" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -758,37 +769,46 @@
         <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>1</v>
       </c>
@@ -805,22 +825,31 @@
         <v>1</v>
       </c>
       <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+      <c r="H2">
         <v>8</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>0</v>
       </c>
-      <c r="L2">
-        <v>2</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>2</v>
+      </c>
+      <c r="P2" t="s">
         <v>36</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -837,22 +866,31 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
+      </c>
+      <c r="I3">
         <v>0</v>
       </c>
-      <c r="L3">
-        <v>2</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
         <v>36</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
@@ -869,22 +907,31 @@
         <v>1</v>
       </c>
       <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
         <v>4</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>0</v>
       </c>
-      <c r="L4">
-        <v>2</v>
-      </c>
-      <c r="M4" t="s">
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4" t="s">
         <v>36</v>
       </c>
-      <c r="O4" t="s">
+      <c r="R4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>2</v>
       </c>
@@ -901,18 +948,27 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
         <v>0</v>
       </c>
-      <c r="L5">
-        <v>2</v>
-      </c>
-      <c r="M5" t="s">
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>2</v>
+      </c>
+      <c r="P5" t="s">
         <v>36</v>
       </c>
-      <c r="O5" t="s">
+      <c r="R5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -930,16 +986,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
-    <col min="5" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.3828125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.15234375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.84375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.3828125" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -953,7 +1009,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -967,7 +1023,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -995,14 +1051,14 @@
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.84375" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1034,7 +1090,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1048,7 +1104,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -1062,7 +1118,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -1076,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -1087,7 +1143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1095,7 +1151,7 @@
         <v>43322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -1103,7 +1159,7 @@
         <v>43323</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1117,7 +1173,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1128,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1142,7 +1198,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1153,7 +1209,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -1170,7 +1226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1181,7 +1237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1192,7 +1248,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
DYNO-23: Handling Parallel Operaitions
updated table structure
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\Work\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91294EA2-5ADA-407E-BA88-F8D1F8D4412C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1D7372-4108-401A-957C-5E0E5F4D756F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -201,13 +201,13 @@
     <t>op4</t>
   </si>
   <si>
-    <t>PrecedingOperation</t>
-  </si>
-  <si>
     <t>WCRuntimeFactor</t>
   </si>
   <si>
     <t>LaborRuntimeFactor</t>
+  </si>
+  <si>
+    <t>PrecedingOperationID</t>
   </si>
 </sst>
 </file>
@@ -576,7 +576,7 @@
   <dimension ref="A1:AMK3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -728,7 +728,7 @@
   <dimension ref="A1:AMN5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -769,16 +769,16 @@
         <v>24</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>25</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>26</v>
@@ -866,7 +866,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -948,7 +948,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>201</v>
       </c>
       <c r="G5">
         <v>1</v>

</xml_diff>

<commit_message>
DYNO-12: Create the basic DB structure for the important tables
Changed the Date format of the excel sheet to yyyy-mm-dd
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\Work\DynoScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC1D7372-4108-401A-957C-5E0E5F4D756F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A4688-79E1-403B-9B3A-C38BADE630D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8194" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -214,8 +214,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -254,11 +255,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -575,36 +578,37 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.3046875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="15.84375" customWidth="1" collapsed="1"/>
-    <col min="3" max="4" width="14.3046875" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="17.3046875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="15.3828125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="16.3828125" style="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.69140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.84375" style="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="23.15234375" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.28515625" style="5" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.28515625" style="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="17.28515625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="15.42578125" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="16.42578125" style="5" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="10.7109375" style="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="11.85546875" style="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="14" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="16.69140625" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="17.15234375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="9.69140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="9.7109375" customWidth="1" collapsed="1"/>
+    <col min="15" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
@@ -616,7 +620,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
@@ -641,14 +645,14 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>43318</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -660,7 +664,7 @@
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="5">
         <v>43403</v>
       </c>
       <c r="J2" t="s">
@@ -679,14 +683,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="5">
         <v>43322</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -698,7 +702,7 @@
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="5">
         <v>43404</v>
       </c>
       <c r="J3" t="s">
@@ -719,7 +723,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -727,32 +731,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMN5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.69140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.69140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="22.69140625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.15234375" customWidth="1" collapsed="1"/>
-    <col min="6" max="7" width="20.15234375" customWidth="1"/>
-    <col min="8" max="8" width="19.53515625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.53515625" customWidth="1"/>
-    <col min="10" max="10" width="13.53515625" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.84375" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="12.15234375" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.15234375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="13.3828125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="8.69140625" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.69140625" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="14.3828125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="15.53515625" customWidth="1" collapsed="1"/>
-    <col min="19" max="1028" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" width="11.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="7" width="20.140625" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="11.85546875" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="12.140625" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="13.140625" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="13.42578125" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="16.7109375" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1" collapsed="1"/>
+    <col min="19" max="1028" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -808,7 +812,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -849,7 +853,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -890,7 +894,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -931,7 +935,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -986,16 +990,16 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.3828125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="16.15234375" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16.84375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.3828125" customWidth="1" collapsed="1"/>
-    <col min="5" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.42578125" customWidth="1" collapsed="1"/>
+    <col min="5" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -1009,7 +1013,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1023,7 +1027,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -1047,22 +1051,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.84375" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="17" customWidth="1" collapsed="1"/>
-    <col min="3" max="1025" width="8.69140625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="17" style="5" customWidth="1" collapsed="1"/>
+    <col min="3" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>33</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>43</v>
       </c>
       <c r="C1" t="s">
@@ -1090,11 +1094,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>43318</v>
       </c>
       <c r="C2">
@@ -1104,11 +1108,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="5">
         <v>43319</v>
       </c>
       <c r="F3">
@@ -1118,11 +1122,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="5">
         <v>43320</v>
       </c>
       <c r="C4">
@@ -1132,38 +1136,38 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5" s="5">
         <v>43321</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="5">
         <v>43322</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7" s="5">
         <v>43323</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="5">
         <v>43324</v>
       </c>
       <c r="D8">
@@ -1173,22 +1177,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9" s="5">
         <v>43318</v>
       </c>
       <c r="J9">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="5">
         <v>43319</v>
       </c>
       <c r="C10">
@@ -1198,22 +1202,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="5">
         <v>43320</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="5">
         <v>43321</v>
       </c>
       <c r="C12">
@@ -1226,33 +1230,33 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13" s="5">
         <v>43322</v>
       </c>
       <c r="H13">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="5">
         <v>43323</v>
       </c>
       <c r="D14">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>41</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15" s="5">
         <v>43324</v>
       </c>
       <c r="G15">

</xml_diff>

<commit_message>
DYNO-22: Update data.xlsx with RevenueValue field
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Prabash\Documents\NetBeansProjects\DynoScheduler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A4688-79E1-403B-9B3A-C38BADE630D2}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFB25929-1D69-45C2-9850-03AE0FF539D6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="650" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ShopOrders" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="WorkCenters" sheetId="3" r:id="rId3"/>
     <sheet name="WorkCenterOpAllocations" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="61">
   <si>
     <t>OrderNo</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>PrecedingOperationID</t>
+  </si>
+  <si>
+    <t>RevenueValue</t>
   </si>
 </sst>
 </file>
@@ -216,7 +219,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd;@"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -260,8 +263,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -601,7 +604,7 @@
     <col min="15" max="1025" width="8.7109375" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -644,8 +647,11 @@
       <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O1" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -682,8 +688,11 @@
       <c r="N2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -719,6 +728,9 @@
       </c>
       <c r="N3" t="s">
         <v>20</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1051,7 +1063,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>

</xml_diff>